<commit_message>
Added date comparisons, is_populated, added code for running in prod
</commit_message>
<xml_diff>
--- a/qc_rules_011823_na_corrected.xlsx
+++ b/qc_rules_011823_na_corrected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersjm/Documents/qaqc_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C08C0DA2-F65F-9E46-9E06-CA82C4FCB696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2A888511-8603-CE4C-A4A0-93A4400BA32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="-400" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qc_rules_011823" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <author>tc={98453098-B2B3-3F45-9641-46A994B7C1FA}</author>
   </authors>
   <commentList>
-    <comment ref="A83" authorId="0" shapeId="1027" xr:uid="{8612CFC9-0F85-1347-A952-BC9EF82FD382}">
+    <comment ref="A83" authorId="0" shapeId="1025" xr:uid="{8612CFC9-0F85-1347-A952-BC9EF82FD382}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -53,21 +53,21 @@
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>81</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>92</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>1511300</xdr:colOff>
-                <xdr:row>85</xdr:row>
-                <xdr:rowOff>139700</xdr:rowOff>
+                <xdr:row>96</xdr:row>
+                <xdr:rowOff>63500</xdr:rowOff>
               </to>
             </anchor>
           </commentPr>
         </mc:Fallback>
       </mc:AlternateContent>
     </comment>
-    <comment ref="A86" authorId="1" shapeId="1025" xr:uid="{55AA35F5-2510-9740-991E-080C522BD670}">
+    <comment ref="A86" authorId="1" shapeId="1026" xr:uid="{55AA35F5-2510-9740-991E-080C522BD670}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,21 +88,21 @@
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>84</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>95</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>1511300</xdr:colOff>
-                <xdr:row>88</xdr:row>
-                <xdr:rowOff>139700</xdr:rowOff>
+                <xdr:row>99</xdr:row>
+                <xdr:rowOff>63500</xdr:rowOff>
               </to>
             </anchor>
           </commentPr>
         </mc:Fallback>
       </mc:AlternateContent>
     </comment>
-    <comment ref="A87" authorId="2" shapeId="1026" xr:uid="{69908563-8959-7F43-8647-5F48029667A4}">
+    <comment ref="A87" authorId="2" shapeId="1027" xr:uid="{69908563-8959-7F43-8647-5F48029667A4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -117,14 +117,14 @@
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>85</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>96</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>1511300</xdr:colOff>
-                <xdr:row>89</xdr:row>
-                <xdr:rowOff>139700</xdr:rowOff>
+                <xdr:row>100</xdr:row>
+                <xdr:rowOff>63500</xdr:rowOff>
               </to>
             </anchor>
           </commentPr>
@@ -146,14 +146,14 @@
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>97</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>108</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>1511300</xdr:colOff>
-                <xdr:row>101</xdr:row>
-                <xdr:rowOff>139700</xdr:rowOff>
+                <xdr:row>112</xdr:row>
+                <xdr:rowOff>63500</xdr:rowOff>
               </to>
             </anchor>
           </commentPr>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1128" uniqueCount="432">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1130" uniqueCount="434">
   <si>
     <t>Qctype</t>
   </si>
@@ -1466,13 +1466,19 @@
   </si>
   <si>
     <t>NA or crossValid3</t>
+  </si>
+  <si>
+    <t>CrossVariableConceptID4</t>
+  </si>
+  <si>
+    <t>CrossVariableConceptID4Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1613,12 +1619,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2035,21 +2035,90 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>84</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:row>92</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1511300</xdr:colOff>
-          <xdr:row>88</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
+          <xdr:row>96</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Comment 1" hidden="1">
+            <xdr:cNvPr id="1025" name="Comment 3" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0940CC5F-8C44-5114-BDE3-B76CFF789277}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91F2564-B9DA-BA6E-8771-E5F82FC50CFF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="3771900" y="20027900"/>
+              <a:ext cx="1320800" cy="876300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFE1" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="80"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="510000"/>
+              </a:solidFill>
+              <a:miter lim="800%"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor editAs="absolute">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>95</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1511300</xdr:colOff>
+          <xdr:row>99</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Comment 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B863F9-446F-8F08-95B9-F6B9619A0D81}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2104,21 +2173,21 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>85</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:row>96</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1511300</xdr:colOff>
-          <xdr:row>89</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
+          <xdr:row>100</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Comment 2" hidden="1">
+            <xdr:cNvPr id="1027" name="Comment 2" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E01CA01F-E46B-011F-2AE5-8671758714A1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AA16AF9-2462-0D7F-227C-9C70145C4F76}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2173,90 +2242,21 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>81</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:row>108</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>1511300</xdr:colOff>
-          <xdr:row>85</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Comment 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11A2FC86-66A9-4885-E1C3-9EE7105DFCD1}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1">
-              <a:spLocks noChangeArrowheads="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="3771900" y="20027900"/>
-              <a:ext cx="1320800" cy="876300"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFE1" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="80"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="510000"/>
-              </a:solidFill>
-              <a:miter lim="800%"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="510000"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
-    <mc:Fallback>
-      <xdr:twoCellAnchor editAs="absolute">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>97</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1511300</xdr:colOff>
-          <xdr:row>101</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
+          <xdr:row>112</xdr:row>
+          <xdr:rowOff>63500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1028" name="Comment 4" hidden="1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17E05BD9-F593-0B9B-61E3-E589A8B1418C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21EF0FA1-7BE7-6539-F4CD-597AC0E7260A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2646,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M179"/>
+  <dimension ref="A1:O179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2664,9 +2664,10 @@
     <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>405</v>
       </c>
@@ -2698,16 +2699,22 @@
         <v>412</v>
       </c>
       <c r="K1" t="s">
+        <v>432</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="M1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2720,14 +2727,14 @@
       <c r="D2" t="s">
         <v>415</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2746,14 +2753,14 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2766,14 +2773,14 @@
       <c r="D4" t="s">
         <v>380</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>6</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2786,11 +2793,11 @@
       <c r="D5" t="s">
         <v>381</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2809,11 +2816,11 @@
       <c r="F6">
         <v>657167265</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2832,11 +2839,11 @@
       <c r="F7">
         <v>548392715</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2855,11 +2862,11 @@
       <c r="F8">
         <v>548392715</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2878,11 +2885,11 @@
       <c r="F9">
         <v>548392715</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="170" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2901,11 +2908,11 @@
       <c r="F10">
         <v>657167265</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2918,11 +2925,11 @@
       <c r="D11" t="s">
         <v>377</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2941,11 +2948,11 @@
       <c r="F12" t="s">
         <v>36</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2964,11 +2971,11 @@
       <c r="F13" t="s">
         <v>40</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2981,14 +2988,14 @@
       <c r="D14">
         <v>25</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>6</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -3007,17 +3014,17 @@
       <c r="F15">
         <v>486306141</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>6</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>49</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -3031,7 +3038,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -3050,17 +3057,17 @@
       <c r="F17">
         <v>486306141</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>6</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>49</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -3074,7 +3081,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -3087,11 +3094,11 @@
       <c r="D19" t="s">
         <v>427</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -3104,14 +3111,14 @@
       <c r="D20" t="s">
         <v>421</v>
       </c>
-      <c r="K20" t="s">
-        <v>60</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -3130,14 +3137,14 @@
       <c r="F21">
         <v>353358909</v>
       </c>
-      <c r="K21" t="s">
-        <v>60</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
+        <v>60</v>
+      </c>
+      <c r="N21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3156,14 +3163,14 @@
       <c r="F22">
         <v>353358909</v>
       </c>
-      <c r="K22" t="s">
-        <v>60</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
+        <v>60</v>
+      </c>
+      <c r="N22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3182,14 +3189,14 @@
       <c r="F23">
         <v>353358909</v>
       </c>
-      <c r="K23" t="s">
-        <v>60</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -3208,14 +3215,14 @@
       <c r="F24">
         <v>353358909</v>
       </c>
-      <c r="K24" t="s">
-        <v>60</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
+        <v>60</v>
+      </c>
+      <c r="N24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3234,14 +3241,14 @@
       <c r="F25">
         <v>353358909</v>
       </c>
-      <c r="K25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
+        <v>60</v>
+      </c>
+      <c r="N25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -3260,14 +3267,14 @@
       <c r="F26">
         <v>353358909</v>
       </c>
-      <c r="K26" t="s">
-        <v>60</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
+        <v>60</v>
+      </c>
+      <c r="N26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -3286,14 +3293,14 @@
       <c r="F27">
         <v>353358910</v>
       </c>
-      <c r="K27" t="s">
-        <v>60</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -3306,14 +3313,14 @@
       <c r="D28">
         <v>800</v>
       </c>
-      <c r="K28" t="s">
-        <v>60</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -3332,14 +3339,14 @@
       <c r="F29">
         <v>353358909</v>
       </c>
-      <c r="K29" t="s">
-        <v>60</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
+        <v>60</v>
+      </c>
+      <c r="N29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -3358,14 +3365,14 @@
       <c r="F30">
         <v>353358909</v>
       </c>
-      <c r="K30" t="s">
-        <v>60</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -3384,14 +3391,14 @@
       <c r="F31">
         <v>353358909</v>
       </c>
-      <c r="K31" t="s">
-        <v>60</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -3410,14 +3417,14 @@
       <c r="F32">
         <v>353358909</v>
       </c>
-      <c r="K32" t="s">
-        <v>60</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
+        <v>60</v>
+      </c>
+      <c r="N32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -3436,14 +3443,14 @@
       <c r="F33">
         <v>353358909</v>
       </c>
-      <c r="K33" t="s">
-        <v>60</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
+        <v>60</v>
+      </c>
+      <c r="N33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -3462,14 +3469,14 @@
       <c r="F34">
         <v>353358909</v>
       </c>
-      <c r="K34" t="s">
-        <v>60</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
+        <v>60</v>
+      </c>
+      <c r="N34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -3488,14 +3495,14 @@
       <c r="F35">
         <v>353358909</v>
       </c>
-      <c r="K35" t="s">
-        <v>60</v>
-      </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
+        <v>60</v>
+      </c>
+      <c r="N35" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -3514,14 +3521,14 @@
       <c r="F36">
         <v>353358909</v>
       </c>
-      <c r="K36" t="s">
-        <v>60</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
+        <v>60</v>
+      </c>
+      <c r="N36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -3540,14 +3547,14 @@
       <c r="F37">
         <v>353358909</v>
       </c>
-      <c r="K37" t="s">
-        <v>60</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
+        <v>60</v>
+      </c>
+      <c r="N37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -3566,14 +3573,14 @@
       <c r="F38">
         <v>353358909</v>
       </c>
-      <c r="K38" t="s">
-        <v>60</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N38" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -3592,14 +3599,14 @@
       <c r="F39">
         <v>353358909</v>
       </c>
-      <c r="K39" t="s">
-        <v>60</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
+        <v>60</v>
+      </c>
+      <c r="N39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -3618,14 +3625,14 @@
       <c r="F40">
         <v>353358909</v>
       </c>
-      <c r="K40" t="s">
-        <v>60</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -3644,14 +3651,14 @@
       <c r="F41">
         <v>353358909</v>
       </c>
-      <c r="K41" t="s">
-        <v>60</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -3670,14 +3677,14 @@
       <c r="F42">
         <v>353358909</v>
       </c>
-      <c r="K42" t="s">
-        <v>60</v>
-      </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3696,14 +3703,14 @@
       <c r="F43">
         <v>353358909</v>
       </c>
-      <c r="K43" t="s">
-        <v>60</v>
-      </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
+        <v>60</v>
+      </c>
+      <c r="N43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -3722,14 +3729,14 @@
       <c r="F44">
         <v>353358909</v>
       </c>
-      <c r="K44" t="s">
-        <v>60</v>
-      </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
+        <v>60</v>
+      </c>
+      <c r="N44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -3748,14 +3755,14 @@
       <c r="F45">
         <v>353358909</v>
       </c>
-      <c r="K45" t="s">
-        <v>60</v>
-      </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
+        <v>60</v>
+      </c>
+      <c r="N45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -3774,14 +3781,14 @@
       <c r="F46">
         <v>353358909</v>
       </c>
-      <c r="K46" t="s">
-        <v>60</v>
-      </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
+        <v>60</v>
+      </c>
+      <c r="N46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>116</v>
       </c>
@@ -3800,14 +3807,14 @@
       <c r="F47">
         <v>353358909</v>
       </c>
-      <c r="K47" t="s">
-        <v>60</v>
-      </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
+        <v>60</v>
+      </c>
+      <c r="N47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -3826,14 +3833,14 @@
       <c r="F48">
         <v>353358909</v>
       </c>
-      <c r="K48" t="s">
-        <v>60</v>
-      </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
+        <v>60</v>
+      </c>
+      <c r="N48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>120</v>
       </c>
@@ -3852,14 +3859,14 @@
       <c r="F49">
         <v>353358909</v>
       </c>
-      <c r="K49" t="s">
-        <v>60</v>
-      </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
+        <v>60</v>
+      </c>
+      <c r="N49" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -3878,14 +3885,14 @@
       <c r="F50">
         <v>353358909</v>
       </c>
-      <c r="K50" t="s">
-        <v>60</v>
-      </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
+        <v>60</v>
+      </c>
+      <c r="N50" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -3904,14 +3911,14 @@
       <c r="F51">
         <v>353358909</v>
       </c>
-      <c r="K51" t="s">
-        <v>60</v>
-      </c>
-      <c r="L51" t="s">
+      <c r="M51" t="s">
+        <v>60</v>
+      </c>
+      <c r="N51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>126</v>
       </c>
@@ -3930,14 +3937,14 @@
       <c r="F52">
         <v>353358909</v>
       </c>
-      <c r="K52" t="s">
-        <v>60</v>
-      </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
+        <v>60</v>
+      </c>
+      <c r="N52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>128</v>
       </c>
@@ -3956,14 +3963,14 @@
       <c r="F53">
         <v>353358909</v>
       </c>
-      <c r="K53" t="s">
-        <v>60</v>
-      </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
+        <v>60</v>
+      </c>
+      <c r="N53" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>130</v>
       </c>
@@ -3982,14 +3989,14 @@
       <c r="F54">
         <v>353358909</v>
       </c>
-      <c r="K54" t="s">
-        <v>60</v>
-      </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
+        <v>60</v>
+      </c>
+      <c r="N54" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -4008,14 +4015,14 @@
       <c r="F55">
         <v>353358909</v>
       </c>
-      <c r="K55" t="s">
-        <v>60</v>
-      </c>
-      <c r="L55" t="s">
+      <c r="M55" t="s">
+        <v>60</v>
+      </c>
+      <c r="N55" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -4028,14 +4035,14 @@
       <c r="D56" t="s">
         <v>421</v>
       </c>
-      <c r="K56" t="s">
+      <c r="M56" t="s">
         <v>6</v>
       </c>
-      <c r="L56" t="s">
+      <c r="N56" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>137</v>
       </c>
@@ -4048,14 +4055,14 @@
       <c r="D57" t="s">
         <v>421</v>
       </c>
-      <c r="K57" t="s">
+      <c r="M57" t="s">
         <v>6</v>
       </c>
-      <c r="L57" t="s">
+      <c r="N57" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -4068,14 +4075,14 @@
       <c r="D58" t="s">
         <v>421</v>
       </c>
-      <c r="K58" t="s">
+      <c r="M58" t="s">
         <v>142</v>
       </c>
-      <c r="L58" t="s">
+      <c r="N58" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>144</v>
       </c>
@@ -4085,14 +4092,14 @@
       <c r="C59" t="s">
         <v>146</v>
       </c>
-      <c r="K59" t="s">
-        <v>60</v>
-      </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
+        <v>60</v>
+      </c>
+      <c r="N59" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>148</v>
       </c>
@@ -4105,11 +4112,11 @@
       <c r="D60" t="s">
         <v>390</v>
       </c>
-      <c r="K60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>150</v>
       </c>
@@ -4122,14 +4129,14 @@
       <c r="D61">
         <v>6</v>
       </c>
-      <c r="K61" t="s">
-        <v>60</v>
-      </c>
-      <c r="L61" t="s">
+      <c r="M61" t="s">
+        <v>60</v>
+      </c>
+      <c r="N61" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>153</v>
       </c>
@@ -4142,14 +4149,14 @@
       <c r="D62" t="s">
         <v>390</v>
       </c>
-      <c r="K62" t="s">
+      <c r="M62" t="s">
         <v>155</v>
       </c>
-      <c r="L62" t="s">
+      <c r="N62" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>157</v>
       </c>
@@ -4168,11 +4175,11 @@
       <c r="F63">
         <v>854703046</v>
       </c>
-      <c r="K63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>159</v>
       </c>
@@ -4185,11 +4192,11 @@
       <c r="D64" t="s">
         <v>390</v>
       </c>
-      <c r="K64" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>161</v>
       </c>
@@ -4202,11 +4209,11 @@
       <c r="D65" t="s">
         <v>390</v>
       </c>
-      <c r="K65" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>163</v>
       </c>
@@ -4219,11 +4226,11 @@
       <c r="D66" t="s">
         <v>390</v>
       </c>
-      <c r="K66" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>165</v>
       </c>
@@ -4236,11 +4243,11 @@
       <c r="D67" t="s">
         <v>390</v>
       </c>
-      <c r="K67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>167</v>
       </c>
@@ -4253,11 +4260,11 @@
       <c r="D68" t="s">
         <v>390</v>
       </c>
-      <c r="K68" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -4270,11 +4277,11 @@
       <c r="D69" t="s">
         <v>390</v>
       </c>
-      <c r="K69" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>171</v>
       </c>
@@ -4287,11 +4294,11 @@
       <c r="D70" t="s">
         <v>390</v>
       </c>
-      <c r="K70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>173</v>
       </c>
@@ -4304,11 +4311,11 @@
       <c r="D71" t="s">
         <v>390</v>
       </c>
-      <c r="K71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>175</v>
       </c>
@@ -4321,11 +4328,11 @@
       <c r="D72" t="s">
         <v>390</v>
       </c>
-      <c r="K72" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -4338,11 +4345,11 @@
       <c r="D73" t="s">
         <v>390</v>
       </c>
-      <c r="K73" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>179</v>
       </c>
@@ -4355,11 +4362,11 @@
       <c r="D74" t="s">
         <v>390</v>
       </c>
-      <c r="K74" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>181</v>
       </c>
@@ -4372,11 +4379,11 @@
       <c r="D75" t="s">
         <v>390</v>
       </c>
-      <c r="K75" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M75" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -4389,11 +4396,11 @@
       <c r="D76" t="s">
         <v>390</v>
       </c>
-      <c r="K76" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>185</v>
       </c>
@@ -4406,11 +4413,11 @@
       <c r="D77" t="s">
         <v>390</v>
       </c>
-      <c r="K77" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M77" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -4423,11 +4430,11 @@
       <c r="D78" t="s">
         <v>390</v>
       </c>
-      <c r="K78" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>189</v>
       </c>
@@ -4440,11 +4447,11 @@
       <c r="D79" t="s">
         <v>390</v>
       </c>
-      <c r="K79" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>191</v>
       </c>
@@ -4457,11 +4464,11 @@
       <c r="D80" t="s">
         <v>390</v>
       </c>
-      <c r="K80" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>193</v>
       </c>
@@ -4474,11 +4481,11 @@
       <c r="D81" t="s">
         <v>390</v>
       </c>
-      <c r="K81" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>195</v>
       </c>
@@ -4491,14 +4498,14 @@
       <c r="D82" t="s">
         <v>390</v>
       </c>
-      <c r="K82" t="s">
+      <c r="M82" t="s">
         <v>6</v>
       </c>
-      <c r="L82" t="s">
+      <c r="N82" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>198</v>
       </c>
@@ -4511,11 +4518,11 @@
       <c r="D83">
         <v>11</v>
       </c>
-      <c r="K83" t="s">
+      <c r="M83" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>200</v>
       </c>
@@ -4534,14 +4541,14 @@
       <c r="F84">
         <v>353358909</v>
       </c>
-      <c r="K84" t="s">
+      <c r="M84" t="s">
         <v>202</v>
       </c>
-      <c r="L84" t="s">
+      <c r="N84" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -4551,14 +4558,14 @@
       <c r="C85" t="s">
         <v>146</v>
       </c>
-      <c r="K85" t="s">
+      <c r="M85" t="s">
         <v>6</v>
       </c>
-      <c r="L85" t="s">
+      <c r="N85" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>205</v>
       </c>
@@ -4571,14 +4578,14 @@
       <c r="D86">
         <v>11</v>
       </c>
-      <c r="K86" t="s">
+      <c r="M86" t="s">
         <v>6</v>
       </c>
-      <c r="L86" t="s">
+      <c r="N86" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>208</v>
       </c>
@@ -4591,14 +4598,14 @@
       <c r="D87">
         <v>50</v>
       </c>
-      <c r="K87" t="s">
+      <c r="M87" t="s">
         <v>6</v>
       </c>
-      <c r="L87" t="s">
+      <c r="N87" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>211</v>
       </c>
@@ -4611,14 +4618,14 @@
       <c r="D88">
         <v>50</v>
       </c>
-      <c r="K88" t="s">
+      <c r="M88" t="s">
         <v>6</v>
       </c>
-      <c r="L88" t="s">
+      <c r="N88" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>214</v>
       </c>
@@ -4631,14 +4638,14 @@
       <c r="D89">
         <v>50</v>
       </c>
-      <c r="K89" t="s">
-        <v>60</v>
-      </c>
-      <c r="L89" t="s">
+      <c r="M89" t="s">
+        <v>60</v>
+      </c>
+      <c r="N89" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>217</v>
       </c>
@@ -4651,14 +4658,14 @@
       <c r="D90" t="s">
         <v>422</v>
       </c>
-      <c r="K90" t="s">
-        <v>60</v>
-      </c>
-      <c r="L90" t="s">
+      <c r="M90" t="s">
+        <v>60</v>
+      </c>
+      <c r="N90" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>220</v>
       </c>
@@ -4668,11 +4675,11 @@
       <c r="C91" t="s">
         <v>222</v>
       </c>
-      <c r="K91" t="s">
+      <c r="M91" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>224</v>
       </c>
@@ -4691,14 +4698,14 @@
       <c r="F92">
         <v>353358909</v>
       </c>
-      <c r="K92" t="s">
+      <c r="M92" t="s">
         <v>223</v>
       </c>
-      <c r="L92" t="s">
+      <c r="N92" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>227</v>
       </c>
@@ -4711,14 +4718,14 @@
       <c r="D93" t="s">
         <v>390</v>
       </c>
-      <c r="K93" t="s">
+      <c r="M93" t="s">
         <v>6</v>
       </c>
-      <c r="L93" t="s">
+      <c r="N93" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>229</v>
       </c>
@@ -4731,11 +4738,11 @@
       <c r="D94">
         <v>240</v>
       </c>
-      <c r="K94" t="s">
+      <c r="M94" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>231</v>
       </c>
@@ -4748,11 +4755,11 @@
       <c r="D95">
         <v>120</v>
       </c>
-      <c r="K95" t="s">
+      <c r="M95" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>234</v>
       </c>
@@ -4765,11 +4772,11 @@
       <c r="D96">
         <v>10</v>
       </c>
-      <c r="L96" t="s">
+      <c r="N96" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>234</v>
       </c>
@@ -4788,14 +4795,14 @@
       <c r="F97" t="s">
         <v>240</v>
       </c>
-      <c r="K97" t="s">
+      <c r="M97" t="s">
         <v>241</v>
       </c>
-      <c r="L97" t="s">
+      <c r="N97" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>243</v>
       </c>
@@ -4808,11 +4815,11 @@
       <c r="D98">
         <v>50</v>
       </c>
-      <c r="K98" t="s">
+      <c r="M98" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>245</v>
       </c>
@@ -4825,11 +4832,11 @@
       <c r="D99" t="s">
         <v>247</v>
       </c>
-      <c r="K99" t="s">
+      <c r="M99" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>208</v>
       </c>
@@ -4842,14 +4849,14 @@
       <c r="D100">
         <v>50</v>
       </c>
-      <c r="K100" t="s">
+      <c r="M100" t="s">
         <v>6</v>
       </c>
-      <c r="L100" t="s">
+      <c r="N100" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>214</v>
       </c>
@@ -4862,14 +4869,14 @@
       <c r="D101">
         <v>1</v>
       </c>
-      <c r="K101" t="s">
-        <v>60</v>
-      </c>
-      <c r="L101" t="s">
+      <c r="M101" t="s">
+        <v>60</v>
+      </c>
+      <c r="N101" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>211</v>
       </c>
@@ -4882,14 +4889,14 @@
       <c r="D102">
         <v>50</v>
       </c>
-      <c r="K102" t="s">
+      <c r="M102" t="s">
         <v>6</v>
       </c>
-      <c r="L102" t="s">
+      <c r="N102" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>217</v>
       </c>
@@ -4902,14 +4909,14 @@
       <c r="D103" t="s">
         <v>422</v>
       </c>
-      <c r="K103" t="s">
-        <v>60</v>
-      </c>
-      <c r="L103" t="s">
+      <c r="M103" t="s">
+        <v>60</v>
+      </c>
+      <c r="N103" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>256</v>
       </c>
@@ -4922,14 +4929,14 @@
       <c r="D104">
         <v>50</v>
       </c>
-      <c r="K104" t="s">
-        <v>60</v>
-      </c>
-      <c r="L104" t="s">
+      <c r="M104" t="s">
+        <v>60</v>
+      </c>
+      <c r="N104" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>259</v>
       </c>
@@ -4942,14 +4949,14 @@
       <c r="D105">
         <v>2</v>
       </c>
-      <c r="K105" t="s">
+      <c r="M105" t="s">
         <v>6</v>
       </c>
-      <c r="L105" t="s">
+      <c r="N105" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>262</v>
       </c>
@@ -4962,14 +4969,14 @@
       <c r="D106">
         <v>2</v>
       </c>
-      <c r="K106" t="s">
+      <c r="M106" t="s">
         <v>6</v>
       </c>
-      <c r="L106" t="s">
+      <c r="N106" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>265</v>
       </c>
@@ -4982,14 +4989,14 @@
       <c r="D107">
         <v>4</v>
       </c>
-      <c r="K107" t="s">
+      <c r="M107" t="s">
         <v>6</v>
       </c>
-      <c r="L107" t="s">
+      <c r="N107" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>268</v>
       </c>
@@ -5002,11 +5009,11 @@
       <c r="D108">
         <v>8</v>
       </c>
-      <c r="K108" t="s">
+      <c r="M108" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>270</v>
       </c>
@@ -5019,11 +5026,11 @@
       <c r="D109">
         <v>3</v>
       </c>
-      <c r="K109" t="s">
+      <c r="M109" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>272</v>
       </c>
@@ -5036,17 +5043,17 @@
       <c r="D110">
         <v>10</v>
       </c>
-      <c r="K110" t="s">
+      <c r="M110" t="s">
         <v>275</v>
       </c>
-      <c r="L110" t="s">
+      <c r="N110" t="s">
         <v>276</v>
       </c>
-      <c r="M110" t="s">
+      <c r="O110" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>278</v>
       </c>
@@ -5065,11 +5072,11 @@
       <c r="F111" t="s">
         <v>281</v>
       </c>
-      <c r="K111" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M111" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>282</v>
       </c>
@@ -5082,11 +5089,11 @@
       <c r="D112" t="s">
         <v>390</v>
       </c>
-      <c r="K112" t="s">
+      <c r="M112" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>284</v>
       </c>
@@ -5099,17 +5106,17 @@
       <c r="D113">
         <v>10</v>
       </c>
-      <c r="K113" t="s">
+      <c r="M113" t="s">
         <v>285</v>
       </c>
-      <c r="L113" t="s">
+      <c r="N113" t="s">
         <v>276</v>
       </c>
-      <c r="M113" t="s">
+      <c r="O113" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>286</v>
       </c>
@@ -5122,11 +5129,11 @@
       <c r="D114" t="s">
         <v>390</v>
       </c>
-      <c r="K114" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M114" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>288</v>
       </c>
@@ -5139,14 +5146,14 @@
       <c r="D115">
         <v>10</v>
       </c>
-      <c r="K115" t="s">
+      <c r="M115" t="s">
         <v>285</v>
       </c>
-      <c r="M115" t="s">
+      <c r="O115" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>290</v>
       </c>
@@ -5159,11 +5166,11 @@
       <c r="D116" t="s">
         <v>390</v>
       </c>
-      <c r="K116" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M116" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>292</v>
       </c>
@@ -5182,14 +5189,14 @@
       <c r="F117">
         <v>353358909</v>
       </c>
-      <c r="K117" t="s">
+      <c r="M117" t="s">
         <v>6</v>
       </c>
-      <c r="M117" t="s">
+      <c r="O117" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>295</v>
       </c>
@@ -5208,14 +5215,14 @@
       <c r="F118">
         <v>353358909</v>
       </c>
-      <c r="K118" t="s">
-        <v>60</v>
-      </c>
       <c r="M118" t="s">
+        <v>60</v>
+      </c>
+      <c r="O118" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>297</v>
       </c>
@@ -5234,14 +5241,14 @@
       <c r="F119">
         <v>353358909</v>
       </c>
-      <c r="K119" t="s">
-        <v>60</v>
-      </c>
       <c r="M119" t="s">
+        <v>60</v>
+      </c>
+      <c r="O119" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>299</v>
       </c>
@@ -5260,14 +5267,14 @@
       <c r="F120">
         <v>353358909</v>
       </c>
-      <c r="K120" t="s">
-        <v>60</v>
-      </c>
       <c r="M120" t="s">
+        <v>60</v>
+      </c>
+      <c r="O120" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>301</v>
       </c>
@@ -5286,14 +5293,14 @@
       <c r="F121">
         <v>353358909</v>
       </c>
-      <c r="K121" t="s">
+      <c r="M121" t="s">
         <v>303</v>
       </c>
-      <c r="L121" t="s">
+      <c r="N121" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>305</v>
       </c>
@@ -5312,17 +5319,17 @@
       <c r="F122">
         <v>353358909</v>
       </c>
-      <c r="K122" t="s">
+      <c r="M122" t="s">
         <v>6</v>
       </c>
-      <c r="L122" t="s">
+      <c r="N122" t="s">
         <v>307</v>
       </c>
-      <c r="M122" t="s">
+      <c r="O122" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>308</v>
       </c>
@@ -5341,17 +5348,17 @@
       <c r="F123">
         <v>353358909</v>
       </c>
-      <c r="K123" t="s">
-        <v>60</v>
-      </c>
-      <c r="L123" t="s">
+      <c r="M123" t="s">
+        <v>60</v>
+      </c>
+      <c r="N123" t="s">
         <v>307</v>
       </c>
-      <c r="M123" t="s">
+      <c r="O123" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>310</v>
       </c>
@@ -5370,17 +5377,17 @@
       <c r="F124">
         <v>353358909</v>
       </c>
-      <c r="K124" t="s">
+      <c r="M124" t="s">
         <v>6</v>
       </c>
-      <c r="L124" t="s">
+      <c r="N124" t="s">
         <v>307</v>
       </c>
-      <c r="M124" t="s">
+      <c r="O124" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>312</v>
       </c>
@@ -5399,17 +5406,17 @@
       <c r="F125">
         <v>353358909</v>
       </c>
-      <c r="K125" t="s">
+      <c r="M125" t="s">
         <v>6</v>
       </c>
-      <c r="L125" t="s">
+      <c r="N125" t="s">
         <v>307</v>
       </c>
-      <c r="M125" t="s">
+      <c r="O125" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>314</v>
       </c>
@@ -5428,17 +5435,17 @@
       <c r="F126">
         <v>353358909</v>
       </c>
-      <c r="K126" t="s">
+      <c r="M126" t="s">
         <v>6</v>
       </c>
-      <c r="L126" t="s">
+      <c r="N126" t="s">
         <v>307</v>
       </c>
-      <c r="M126" t="s">
+      <c r="O126" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>316</v>
       </c>
@@ -5457,11 +5464,11 @@
       <c r="F127">
         <v>353358909</v>
       </c>
-      <c r="K127" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M127" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>318</v>
       </c>
@@ -5474,14 +5481,14 @@
       <c r="D128">
         <v>4</v>
       </c>
-      <c r="K128" t="s">
-        <v>60</v>
-      </c>
-      <c r="L128" t="s">
+      <c r="M128" t="s">
+        <v>60</v>
+      </c>
+      <c r="N128" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>321</v>
       </c>
@@ -5494,17 +5501,17 @@
       <c r="D129">
         <v>800</v>
       </c>
-      <c r="K129" t="s">
-        <v>60</v>
-      </c>
-      <c r="L129" t="s">
+      <c r="M129" t="s">
+        <v>60</v>
+      </c>
+      <c r="N129" t="s">
         <v>323</v>
       </c>
-      <c r="M129" t="s">
+      <c r="O129" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>324</v>
       </c>
@@ -5517,17 +5524,17 @@
       <c r="D130">
         <v>800</v>
       </c>
-      <c r="K130" t="s">
-        <v>60</v>
-      </c>
-      <c r="L130" t="s">
+      <c r="M130" t="s">
+        <v>60</v>
+      </c>
+      <c r="N130" t="s">
         <v>323</v>
       </c>
-      <c r="M130" t="s">
+      <c r="O130" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>326</v>
       </c>
@@ -5540,11 +5547,11 @@
       <c r="D131" t="s">
         <v>390</v>
       </c>
-      <c r="K131" t="s">
+      <c r="M131" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>327</v>
       </c>
@@ -5557,14 +5564,14 @@
       <c r="D132">
         <v>24</v>
       </c>
-      <c r="K132" t="s">
+      <c r="M132" t="s">
         <v>329</v>
       </c>
-      <c r="L132" t="s">
+      <c r="N132" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>330</v>
       </c>
@@ -5577,14 +5584,14 @@
       <c r="D133">
         <v>18</v>
       </c>
-      <c r="K133" t="s">
+      <c r="M133" t="s">
         <v>6</v>
       </c>
-      <c r="L133" t="s">
+      <c r="N133" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>333</v>
       </c>
@@ -5597,14 +5604,14 @@
       <c r="D134">
         <v>18</v>
       </c>
-      <c r="K134" t="s">
+      <c r="M134" t="s">
         <v>6</v>
       </c>
-      <c r="L134" t="s">
+      <c r="N134" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>335</v>
       </c>
@@ -5617,14 +5624,14 @@
       <c r="D135" t="s">
         <v>424</v>
       </c>
-      <c r="K135" t="s">
+      <c r="M135" t="s">
         <v>6</v>
       </c>
-      <c r="L135" t="s">
+      <c r="N135" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>338</v>
       </c>
@@ -5637,14 +5644,14 @@
       <c r="D136">
         <v>24</v>
       </c>
-      <c r="K136" t="s">
+      <c r="M136" t="s">
         <v>340</v>
       </c>
-      <c r="L136" t="s">
+      <c r="N136" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>341</v>
       </c>
@@ -5657,14 +5664,14 @@
       <c r="D137">
         <v>2</v>
       </c>
-      <c r="K137" t="s">
+      <c r="M137" t="s">
         <v>340</v>
       </c>
-      <c r="L137" t="s">
+      <c r="N137" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>344</v>
       </c>
@@ -5677,14 +5684,14 @@
       <c r="D138" t="s">
         <v>388</v>
       </c>
-      <c r="K138" t="s">
+      <c r="M138" t="s">
         <v>6</v>
       </c>
-      <c r="L138" t="s">
+      <c r="N138" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>347</v>
       </c>
@@ -5697,14 +5704,14 @@
       <c r="D139" t="s">
         <v>390</v>
       </c>
-      <c r="K139" t="s">
+      <c r="M139" t="s">
         <v>6</v>
       </c>
-      <c r="L139" t="s">
+      <c r="N139" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>350</v>
       </c>
@@ -5717,14 +5724,14 @@
       <c r="D140" t="s">
         <v>388</v>
       </c>
-      <c r="K140" t="s">
+      <c r="M140" t="s">
         <v>6</v>
       </c>
-      <c r="L140" t="s">
+      <c r="N140" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>352</v>
       </c>
@@ -5737,14 +5744,14 @@
       <c r="D141" t="s">
         <v>425</v>
       </c>
-      <c r="K141" t="s">
+      <c r="M141" t="s">
         <v>354</v>
       </c>
-      <c r="L141" t="s">
+      <c r="N141" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>355</v>
       </c>
@@ -5763,14 +5770,14 @@
       <c r="F142">
         <v>922622075</v>
       </c>
-      <c r="K142" t="s">
+      <c r="M142" t="s">
         <v>6</v>
       </c>
-      <c r="L142" t="s">
+      <c r="N142" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>357</v>
       </c>
@@ -5783,14 +5790,14 @@
       <c r="D143" t="s">
         <v>393</v>
       </c>
-      <c r="K143" t="s">
+      <c r="M143" t="s">
         <v>6</v>
       </c>
-      <c r="L143" t="s">
+      <c r="N143" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>359</v>
       </c>
@@ -5803,14 +5810,14 @@
       <c r="D144" t="s">
         <v>393</v>
       </c>
-      <c r="K144" t="s">
+      <c r="M144" t="s">
         <v>6</v>
       </c>
-      <c r="L144" t="s">
+      <c r="N144" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>361</v>
       </c>
@@ -5823,14 +5830,14 @@
       <c r="D145" t="s">
         <v>393</v>
       </c>
-      <c r="K145" t="s">
+      <c r="M145" t="s">
         <v>6</v>
       </c>
-      <c r="L145" t="s">
+      <c r="N145" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>363</v>
       </c>
@@ -5843,14 +5850,14 @@
       <c r="D146" t="s">
         <v>393</v>
       </c>
-      <c r="K146" t="s">
+      <c r="M146" t="s">
         <v>365</v>
       </c>
-      <c r="L146" t="s">
+      <c r="N146" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>367</v>
       </c>
@@ -5869,14 +5876,14 @@
       <c r="F147" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="K147" t="s">
+      <c r="M147" t="s">
         <v>365</v>
       </c>
-      <c r="L147" t="s">
+      <c r="N147" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>352</v>
       </c>
@@ -5895,11 +5902,11 @@
       <c r="F148">
         <v>922622075</v>
       </c>
-      <c r="M148" t="s">
+      <c r="O148" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>352</v>
       </c>
@@ -5918,11 +5925,11 @@
       <c r="F149" t="s">
         <v>373</v>
       </c>
-      <c r="M149" t="s">
+      <c r="O149" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>375</v>
       </c>
@@ -5941,11 +5948,11 @@
       <c r="F150">
         <v>426360242</v>
       </c>
-      <c r="M150" t="s">
+      <c r="O150" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>32</v>
       </c>
@@ -5970,11 +5977,11 @@
       <c r="H151" t="s">
         <v>378</v>
       </c>
-      <c r="M151" t="s">
+      <c r="O151" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>14</v>
       </c>
@@ -5999,11 +6006,11 @@
       <c r="H152" t="s">
         <v>378</v>
       </c>
-      <c r="M152" t="s">
+      <c r="O152" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>17</v>
       </c>
@@ -6028,11 +6035,11 @@
       <c r="H153" t="s">
         <v>378</v>
       </c>
-      <c r="M153" t="s">
+      <c r="O153" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>19</v>
       </c>
@@ -6063,11 +6070,11 @@
       <c r="J154" t="s">
         <v>378</v>
       </c>
-      <c r="M154" t="s">
+      <c r="O154" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>23</v>
       </c>
@@ -6098,11 +6105,11 @@
       <c r="J155" t="s">
         <v>378</v>
       </c>
-      <c r="M155" t="s">
+      <c r="O155" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>34</v>
       </c>
@@ -6133,11 +6140,11 @@
       <c r="J156" t="s">
         <v>378</v>
       </c>
-      <c r="M156" t="s">
+      <c r="O156" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>38</v>
       </c>
@@ -6168,11 +6175,11 @@
       <c r="J157" t="s">
         <v>378</v>
       </c>
-      <c r="M157" t="s">
+      <c r="O157" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>344</v>
       </c>
@@ -6197,11 +6204,11 @@
       <c r="H158" t="s">
         <v>378</v>
       </c>
-      <c r="M158" t="s">
+      <c r="O158" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>347</v>
       </c>
@@ -6226,11 +6233,11 @@
       <c r="H159" t="s">
         <v>378</v>
       </c>
-      <c r="M159" t="s">
+      <c r="O159" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>350</v>
       </c>
@@ -6255,11 +6262,11 @@
       <c r="H160" t="s">
         <v>378</v>
       </c>
-      <c r="M160" t="s">
+      <c r="O160" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>352</v>
       </c>
@@ -6284,11 +6291,11 @@
       <c r="H161" t="s">
         <v>378</v>
       </c>
-      <c r="M161" t="s">
+      <c r="O161" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>355</v>
       </c>
@@ -6313,11 +6320,11 @@
       <c r="H162" t="s">
         <v>378</v>
       </c>
-      <c r="M162" t="s">
+      <c r="O162" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>357</v>
       </c>
@@ -6342,11 +6349,11 @@
       <c r="H163" t="s">
         <v>378</v>
       </c>
-      <c r="M163" t="s">
+      <c r="O163" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>359</v>
       </c>
@@ -6371,11 +6378,11 @@
       <c r="H164" t="s">
         <v>378</v>
       </c>
-      <c r="M164" t="s">
+      <c r="O164" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>361</v>
       </c>
@@ -6400,11 +6407,11 @@
       <c r="H165" t="s">
         <v>378</v>
       </c>
-      <c r="M165" t="s">
+      <c r="O165" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>363</v>
       </c>
@@ -6429,11 +6436,11 @@
       <c r="H166" t="s">
         <v>378</v>
       </c>
-      <c r="M166" t="s">
+      <c r="O166" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>367</v>
       </c>
@@ -6458,11 +6465,11 @@
       <c r="H167" t="s">
         <v>378</v>
       </c>
-      <c r="M167" t="s">
+      <c r="O167" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>394</v>
       </c>
@@ -6487,11 +6494,11 @@
       <c r="H168" t="s">
         <v>378</v>
       </c>
-      <c r="M168" t="s">
+      <c r="O168" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>396</v>
       </c>
@@ -6516,11 +6523,11 @@
       <c r="H169" t="s">
         <v>378</v>
       </c>
-      <c r="M169" t="s">
+      <c r="O169" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>399</v>
       </c>
@@ -6545,11 +6552,11 @@
       <c r="H170" t="s">
         <v>378</v>
       </c>
-      <c r="M170" t="s">
+      <c r="O170" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>401</v>
       </c>
@@ -6574,11 +6581,11 @@
       <c r="H171" t="s">
         <v>378</v>
       </c>
-      <c r="M171" t="s">
+      <c r="O171" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>19</v>
       </c>
@@ -6603,11 +6610,11 @@
       <c r="H172">
         <v>486306141</v>
       </c>
-      <c r="M172" t="s">
+      <c r="O172" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>23</v>
       </c>
@@ -6632,11 +6639,11 @@
       <c r="H173">
         <v>486306141</v>
       </c>
-      <c r="M173" t="s">
+      <c r="O173" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>34</v>
       </c>
@@ -6661,11 +6668,11 @@
       <c r="H174">
         <v>486306141</v>
       </c>
-      <c r="M174" t="s">
+      <c r="O174" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>38</v>
       </c>
@@ -6690,11 +6697,11 @@
       <c r="H175">
         <v>486306141</v>
       </c>
-      <c r="M175" t="s">
+      <c r="O175" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>19</v>
       </c>
@@ -6725,11 +6732,11 @@
       <c r="J176">
         <v>197316935</v>
       </c>
-      <c r="M176" t="s">
+      <c r="O176" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>23</v>
       </c>
@@ -6760,11 +6767,11 @@
       <c r="J177">
         <v>197316935</v>
       </c>
-      <c r="M177" t="s">
+      <c r="O177" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>34</v>
       </c>
@@ -6795,11 +6802,11 @@
       <c r="J178">
         <v>197316935</v>
       </c>
-      <c r="M178" t="s">
+      <c r="O178" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>38</v>
       </c>
@@ -6830,7 +6837,7 @@
       <c r="J179">
         <v>197316935</v>
       </c>
-      <c r="M179" t="s">
+      <c r="O179" t="s">
         <v>404</v>
       </c>
     </row>

</xml_diff>